<commit_message>
ln arreglado , borrado de exp
</commit_message>
<xml_diff>
--- a/Automata/Matriz_de_transicion.xlsx
+++ b/Automata/Matriz_de_transicion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megui\OneDrive\Documentos\GitHub\Compiladores\Automata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA827D-7EF4-421D-A042-45CF98D4264C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1460F7-E1D4-4FC8-8457-CF62A9D15D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="29">
   <si>
     <t>.</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Otro</t>
   </si>
   <si>
-    <t>};</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -116,7 +113,13 @@
     <t>{2,</t>
   </si>
   <si>
-    <t>int automata [][30]{</t>
+    <t>l</t>
+  </si>
+  <si>
+    <t>int automata [][31]{</t>
+  </si>
+  <si>
+    <t>}:</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BJ70"/>
+  <dimension ref="A1:BK70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM22" sqref="AM22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AQ20" sqref="AQ20:AQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,24 +599,26 @@
         <v>13</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="AE1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AF1" s="1"/>
     </row>
     <row r="2" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -709,7 +714,9 @@
       <c r="AE2" s="2">
         <v>22</v>
       </c>
-      <c r="AF2" s="1"/>
+      <c r="AF2" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -805,7 +812,9 @@
       <c r="AE3" s="2">
         <v>4</v>
       </c>
-      <c r="AF3" s="1"/>
+      <c r="AF3" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -901,7 +910,9 @@
       <c r="AE4" s="2">
         <v>4</v>
       </c>
-      <c r="AF4" s="1"/>
+      <c r="AF4" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -997,7 +1008,9 @@
       <c r="AE5" s="2">
         <v>5</v>
       </c>
-      <c r="AF5" s="1"/>
+      <c r="AF5" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -1093,7 +1106,9 @@
       <c r="AE6" s="2">
         <v>0</v>
       </c>
-      <c r="AF6" s="1"/>
+      <c r="AF6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1189,7 +1204,9 @@
       <c r="AE7" s="2">
         <v>0</v>
       </c>
-      <c r="AF7" s="1"/>
+      <c r="AF7" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1279,13 +1296,15 @@
       <c r="AC8">
         <v>0</v>
       </c>
-      <c r="AD8">
+      <c r="AD8" s="2">
         <v>0</v>
       </c>
       <c r="AE8" s="2">
         <v>0</v>
       </c>
-      <c r="AF8" s="1"/>
+      <c r="AF8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1373,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="AC9" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AD9" s="2">
         <v>0</v>
@@ -1381,7 +1400,9 @@
       <c r="AE9" s="2">
         <v>0</v>
       </c>
-      <c r="AF9" s="1"/>
+      <c r="AF9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1471,13 +1492,15 @@
       <c r="AC10">
         <v>0</v>
       </c>
-      <c r="AD10">
+      <c r="AD10" s="2">
         <v>0</v>
       </c>
       <c r="AE10" s="2">
         <v>0</v>
       </c>
-      <c r="AF10" s="1"/>
+      <c r="AF10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1573,7 +1596,9 @@
       <c r="AE11" s="2">
         <v>0</v>
       </c>
-      <c r="AF11" s="1"/>
+      <c r="AF11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1663,13 +1688,15 @@
       <c r="AC12">
         <v>0</v>
       </c>
-      <c r="AD12">
+      <c r="AD12" s="2">
         <v>0</v>
       </c>
       <c r="AE12" s="2">
         <v>0</v>
       </c>
-      <c r="AF12" s="1"/>
+      <c r="AF12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1765,7 +1792,9 @@
       <c r="AE13" s="2">
         <v>0</v>
       </c>
-      <c r="AF13" s="1"/>
+      <c r="AF13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1855,13 +1884,15 @@
       <c r="AC14">
         <v>0</v>
       </c>
-      <c r="AD14">
+      <c r="AD14" s="2">
         <v>0</v>
       </c>
       <c r="AE14" s="2">
         <v>0</v>
       </c>
-      <c r="AF14" s="1"/>
+      <c r="AF14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1957,7 +1988,9 @@
       <c r="AE15" s="2">
         <v>0</v>
       </c>
-      <c r="AF15" s="1"/>
+      <c r="AF15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -2047,15 +2080,17 @@
       <c r="AC16">
         <v>0</v>
       </c>
-      <c r="AD16">
+      <c r="AD16" s="2">
         <v>0</v>
       </c>
       <c r="AE16" s="2">
         <v>0</v>
       </c>
-      <c r="AF16" s="1"/>
+      <c r="AF16" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2149,9 +2184,11 @@
       <c r="AE17" s="2">
         <v>0</v>
       </c>
-      <c r="AF17" s="1"/>
+      <c r="AF17" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2245,9 +2282,11 @@
       <c r="AE18" s="2">
         <v>0</v>
       </c>
-      <c r="AF18" s="1"/>
+      <c r="AF18" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2341,9 +2380,12 @@
       <c r="AE19" s="2">
         <v>0</v>
       </c>
-      <c r="AF19" s="1"/>
+      <c r="AF19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="3"/>
     </row>
-    <row r="20" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2434,11 +2476,14 @@
       <c r="AD20" s="1">
         <v>0</v>
       </c>
-      <c r="AE20" s="1">
+      <c r="AE20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2500,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="U21" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="V21" s="1">
         <v>0</v>
@@ -2532,8 +2577,11 @@
       <c r="AE21" s="2">
         <v>0</v>
       </c>
+      <c r="AF21" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2627,9 +2675,12 @@
       <c r="AE22" s="2">
         <v>0</v>
       </c>
+      <c r="AF22" s="2">
+        <v>0</v>
+      </c>
       <c r="AY22" s="3"/>
     </row>
-    <row r="23" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2723,117 +2774,218 @@
       <c r="AE23" s="2">
         <v>0</v>
       </c>
+      <c r="AF23" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="K24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="O24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="P24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="R24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="S24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="T24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="U24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="V24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="W24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="X24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AA24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AD24" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AE24" s="1">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AA25" s="1"/>
+    <row r="25" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <v>23</v>
+      </c>
+      <c r="D25" s="1">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1">
+        <v>23</v>
+      </c>
+      <c r="F25" s="1">
+        <v>23</v>
+      </c>
+      <c r="G25" s="1">
+        <v>23</v>
+      </c>
+      <c r="H25" s="1">
+        <v>23</v>
+      </c>
+      <c r="I25" s="1">
+        <v>23</v>
+      </c>
+      <c r="J25" s="1">
+        <v>23</v>
+      </c>
+      <c r="K25" s="1">
+        <v>23</v>
+      </c>
+      <c r="L25" s="1">
+        <v>23</v>
+      </c>
+      <c r="M25" s="1">
+        <v>23</v>
+      </c>
+      <c r="N25" s="1">
+        <v>23</v>
+      </c>
+      <c r="O25" s="1">
+        <v>23</v>
+      </c>
+      <c r="P25" s="1">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>23</v>
+      </c>
+      <c r="R25" s="1">
+        <v>23</v>
+      </c>
+      <c r="S25" s="1">
+        <v>23</v>
+      </c>
+      <c r="T25" s="1">
+        <v>23</v>
+      </c>
+      <c r="U25" s="1">
+        <v>23</v>
+      </c>
+      <c r="V25" s="1">
+        <v>23</v>
+      </c>
+      <c r="W25" s="1">
+        <v>23</v>
+      </c>
+      <c r="X25" s="1">
+        <v>23</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE25" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>23</v>
+      </c>
     </row>
-    <row r="26" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1"/>
     </row>
-    <row r="27" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA27" s="1"/>
       <c r="AF27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1"/>
@@ -2904,70 +3056,74 @@
         <v>14,</v>
       </c>
       <c r="AW28" s="1" t="str">
-        <f t="shared" ref="AW28:AW50" si="1">R2&amp;","</f>
+        <f t="shared" ref="AW28:AW51" si="1">R2&amp;","</f>
         <v>12,</v>
       </c>
       <c r="AX28" s="1" t="str">
-        <f t="shared" ref="AX28:AX50" si="2">S2&amp;","</f>
+        <f t="shared" ref="AX28:AX51" si="2">S2&amp;","</f>
         <v>13,</v>
       </c>
       <c r="AY28" s="1" t="str">
-        <f t="shared" ref="AY28:AY50" si="3">T2&amp;","</f>
+        <f t="shared" ref="AY28:AY51" si="3">T2&amp;","</f>
         <v>6,</v>
       </c>
       <c r="AZ28" s="1" t="str">
-        <f t="shared" ref="AZ28:AZ50" si="4">U2&amp;","</f>
+        <f t="shared" ref="AZ28:AZ51" si="4">U2&amp;","</f>
         <v>7,</v>
       </c>
       <c r="BA28" s="1" t="str">
-        <f t="shared" ref="BA28:BA50" si="5">V2&amp;","</f>
+        <f t="shared" ref="BA28:BA51" si="5">V2&amp;","</f>
         <v>15,</v>
       </c>
       <c r="BB28" s="1" t="str">
-        <f t="shared" ref="BB28:BB50" si="6">W2&amp;","</f>
+        <f t="shared" ref="BB28:BB51" si="6">W2&amp;","</f>
         <v>0,</v>
       </c>
       <c r="BC28" s="1" t="str">
-        <f t="shared" ref="BC28:BC50" si="7">X2&amp;","</f>
+        <f t="shared" ref="BC28:BC51" si="7">X2&amp;","</f>
         <v>0,</v>
       </c>
       <c r="BD28" s="1" t="str">
-        <f t="shared" ref="BD28:BD50" si="8">Y2&amp;","</f>
+        <f t="shared" ref="BD28:BD51" si="8">Y2&amp;","</f>
         <v>16,</v>
       </c>
       <c r="BE28" s="1" t="str">
-        <f t="shared" ref="BE28:BE50" si="9">Z2&amp;","</f>
+        <f t="shared" ref="BE28:BE51" si="9">Z2&amp;","</f>
         <v>17,</v>
       </c>
       <c r="BF28" s="1" t="str">
-        <f t="shared" ref="BF28:BF50" si="10">AA2&amp;","</f>
+        <f t="shared" ref="BF28:BF51" si="10">AA2&amp;","</f>
         <v>18,</v>
       </c>
       <c r="BG28" s="1" t="str">
-        <f t="shared" ref="BG28:BG50" si="11">AB2&amp;","</f>
+        <f t="shared" ref="BG28:BG51" si="11">AB2&amp;","</f>
         <v>19,</v>
       </c>
       <c r="BH28" s="1" t="str">
-        <f t="shared" ref="BH28:BH50" si="12">AC2&amp;","</f>
+        <f t="shared" ref="BH28:BH51" si="12">AC2&amp;","</f>
         <v>20,</v>
       </c>
       <c r="BI28" s="1" t="str">
-        <f t="shared" ref="BI28:BI50" si="13">AD2&amp;","</f>
+        <f t="shared" ref="BI28:BI51" si="13">AD2&amp;","</f>
         <v>21,</v>
       </c>
-      <c r="BJ28" s="1" t="str">
-        <f>AE2&amp;"}"&amp;","</f>
-        <v>22},</v>
+      <c r="BJ28" s="1">
+        <f>AE2</f>
+        <v>22</v>
+      </c>
+      <c r="BK28" s="1" t="str">
+        <f>AF2&amp;"}"&amp;","</f>
+        <v>23},</v>
       </c>
     </row>
-    <row r="29" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
       <c r="AF29" s="1"/>
       <c r="AG29" s="1" t="str">
-        <f t="shared" ref="AG29:AG50" si="14">"{"&amp;B3&amp;","</f>
+        <f t="shared" ref="AG29:AG51" si="14">"{"&amp;B3&amp;","</f>
         <v>{1,</v>
       </c>
       <c r="AH29" s="1" t="str">
@@ -3023,11 +3179,11 @@
         <v>4,</v>
       </c>
       <c r="AU29" s="1" t="str">
-        <f t="shared" ref="AU29:AU50" si="15">P3&amp;","</f>
+        <f t="shared" ref="AU29:AU51" si="15">P3&amp;","</f>
         <v>4,</v>
       </c>
       <c r="AV29" s="1" t="str">
-        <f t="shared" ref="AV29:AV50" si="16">Q3&amp;","</f>
+        <f t="shared" ref="AV29:AV51" si="16">Q3&amp;","</f>
         <v>4,</v>
       </c>
       <c r="AW29" s="1" t="str">
@@ -3082,12 +3238,16 @@
         <f t="shared" si="13"/>
         <v>4,</v>
       </c>
-      <c r="BJ29" s="1" t="str">
-        <f t="shared" ref="BJ29:BJ50" si="17">AE3&amp;"}"&amp;","</f>
+      <c r="BJ29" s="1">
+        <f t="shared" ref="BJ29:BJ51" si="17">AE3</f>
+        <v>4</v>
+      </c>
+      <c r="BK29" s="1" t="str">
+        <f t="shared" ref="BK29:BK51" si="18">AF3&amp;"}"&amp;","</f>
         <v>4},</v>
       </c>
     </row>
-    <row r="30" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA30" s="1"/>
       <c r="AG30" s="1" t="str">
         <f t="shared" si="14"/>
@@ -3205,12 +3365,16 @@
         <f t="shared" si="13"/>
         <v>4,</v>
       </c>
-      <c r="BJ30" s="1" t="str">
+      <c r="BJ30" s="1">
         <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="BK30" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>4},</v>
       </c>
     </row>
-    <row r="31" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA31" s="1"/>
       <c r="AG31" s="1" t="str">
         <f t="shared" si="14"/>
@@ -3328,12 +3492,16 @@
         <f t="shared" si="13"/>
         <v>5,</v>
       </c>
-      <c r="BJ31" s="1" t="str">
+      <c r="BJ31" s="1">
         <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="BK31" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>5},</v>
       </c>
     </row>
-    <row r="32" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA32" s="1"/>
       <c r="AG32" s="1" t="str">
         <f t="shared" si="14"/>
@@ -3451,12 +3619,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ32" s="1" t="str">
+      <c r="BJ32" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK32" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="33" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA33" s="1"/>
       <c r="AG33" s="1" t="str">
         <f t="shared" si="14"/>
@@ -3574,12 +3746,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ33" s="1" t="str">
+      <c r="BJ33" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK33" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="34" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AG34" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
@@ -3696,12 +3872,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ34" s="1" t="str">
+      <c r="BJ34" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK34" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="35" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA35" s="1"/>
       <c r="AG35" s="1" t="str">
         <f t="shared" si="14"/>
@@ -3813,18 +3993,22 @@
       </c>
       <c r="BH35" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>20,</v>
+        <v>0,</v>
       </c>
       <c r="BI35" s="1" t="str">
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ35" s="1" t="str">
+      <c r="BJ35" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK35" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="36" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA36" s="1"/>
       <c r="AG36" s="1" t="str">
         <f t="shared" si="14"/>
@@ -3942,12 +4126,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ36" s="1" t="str">
+      <c r="BJ36" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK36" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="37" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA37" s="1"/>
       <c r="AG37" s="1" t="str">
         <f t="shared" si="14"/>
@@ -4065,12 +4253,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ37" s="1" t="str">
+      <c r="BJ37" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK37" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="38" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA38" s="1"/>
       <c r="AG38" s="1" t="str">
         <f t="shared" si="14"/>
@@ -4188,12 +4380,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ38" s="1" t="str">
+      <c r="BJ38" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK38" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="39" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA39" s="1"/>
       <c r="AG39" s="1" t="str">
         <f t="shared" si="14"/>
@@ -4311,12 +4507,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ39" s="1" t="str">
+      <c r="BJ39" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK39" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="40" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AG40" s="1" t="str">
@@ -4435,12 +4635,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ40" s="1" t="str">
+      <c r="BJ40" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK40" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="41" spans="27:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="27:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AG41" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
@@ -4557,12 +4761,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ41" s="1" t="str">
+      <c r="BJ41" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK41" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="42" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="42" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG42" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
@@ -4679,12 +4887,16 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ42" s="1" t="str">
+      <c r="BJ42" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK42" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="43" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="43" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG43" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
@@ -4801,66 +5013,70 @@
         <f t="shared" si="13"/>
         <v>21,</v>
       </c>
-      <c r="BJ43" s="1" t="str">
+      <c r="BJ43" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK43" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="44" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="44" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG44" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
       </c>
       <c r="AH44" s="1" t="str">
-        <f t="shared" ref="AH44:AT50" si="18">C18&amp;","</f>
+        <f t="shared" ref="AH44:AT51" si="19">C18&amp;","</f>
         <v>0,</v>
       </c>
       <c r="AI44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AJ44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AK44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AL44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AM44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AN44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AO44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AP44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AQ44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AR44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AS44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AT44" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AU44" s="1" t="str">
@@ -4923,66 +5139,70 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ44" s="1" t="str">
+      <c r="BJ44" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK44" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="45" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="45" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG45" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
       </c>
       <c r="AH45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AI45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AJ45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AK45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AL45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AM45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AN45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AO45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AP45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AQ45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AR45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AS45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AT45" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AU45" s="1" t="str">
@@ -5045,66 +5265,70 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ45" s="1" t="str">
+      <c r="BJ45" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK45" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="46" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="46" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG46" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
       </c>
       <c r="AH46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AI46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AJ46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AK46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AL46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AM46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AN46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AO46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AP46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AQ46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AR46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AS46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AT46" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AU46" s="1" t="str">
@@ -5167,66 +5391,70 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ46" s="1" t="str">
+      <c r="BJ46" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK46" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="47" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="47" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG47" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
       </c>
       <c r="AH47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AI47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AJ47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AK47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AL47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AM47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AN47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AO47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AP47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AQ47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AR47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AS47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AT47" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AU47" s="1" t="str">
@@ -5251,7 +5479,7 @@
       </c>
       <c r="AZ47" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>7,</v>
+        <v>0,</v>
       </c>
       <c r="BA47" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5289,66 +5517,70 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ47" s="1" t="str">
+      <c r="BJ47" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK47" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="48" spans="27:62" x14ac:dyDescent="0.25">
+    <row r="48" spans="27:63" x14ac:dyDescent="0.25">
       <c r="AG48" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
       </c>
       <c r="AH48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AI48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AJ48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AK48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AL48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AM48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AN48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AO48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AP48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AQ48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AR48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AS48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AT48" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AU48" s="1" t="str">
@@ -5411,66 +5643,70 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ48" s="1" t="str">
+      <c r="BJ48" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK48" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="49" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:63" x14ac:dyDescent="0.25">
       <c r="AG49" s="1" t="str">
         <f t="shared" si="14"/>
         <v>{0,</v>
       </c>
       <c r="AH49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AI49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AJ49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AK49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AL49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AM49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AN49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AO49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AP49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AQ49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AR49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AS49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AT49" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0,</v>
       </c>
       <c r="AU49" s="1" t="str">
@@ -5533,1224 +5769,1355 @@
         <f t="shared" si="13"/>
         <v>0,</v>
       </c>
-      <c r="BJ49" s="1" t="str">
+      <c r="BJ49" s="1">
         <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BK49" s="1" t="str">
+        <f t="shared" si="18"/>
         <v>0},</v>
       </c>
     </row>
-    <row r="50" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:63" x14ac:dyDescent="0.25">
       <c r="AG50" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>{22,</v>
+        <v>{0,</v>
       </c>
       <c r="AH50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AI50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AJ50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AK50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AL50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AM50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AN50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AO50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AP50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AQ50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AR50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AS50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AT50" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>22,</v>
+        <f t="shared" si="19"/>
+        <v>0,</v>
       </c>
       <c r="AU50" s="1" t="str">
         <f t="shared" si="15"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="AV50" s="1" t="str">
         <f t="shared" si="16"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="AW50" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="AX50" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="AY50" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="AZ50" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BA50" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BB50" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BC50" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BD50" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BE50" s="1" t="str">
         <f t="shared" si="9"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BF50" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BG50" s="1" t="str">
         <f t="shared" si="11"/>
-        <v>22,</v>
+        <v>0,</v>
       </c>
       <c r="BH50" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>22,</v>
+        <v>20,</v>
       </c>
       <c r="BI50" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>22,</v>
-      </c>
-      <c r="BJ50" s="1" t="str">
+        <v>0,</v>
+      </c>
+      <c r="BJ50" s="1">
         <f t="shared" si="17"/>
-        <v>22},</v>
+        <v>0</v>
+      </c>
+      <c r="BK50" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0},</v>
       </c>
     </row>
-    <row r="51" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="AF51" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK51" s="1"/>
+    <row r="51" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="AG51" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>{23,</v>
+      </c>
+      <c r="AH51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AI51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AJ51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AK51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AL51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AM51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AN51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AO51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AP51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AQ51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AR51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AS51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AT51" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>23,</v>
+      </c>
+      <c r="AU51" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>23,</v>
+      </c>
+      <c r="AV51" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>23,</v>
+      </c>
+      <c r="AW51" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>23,</v>
+      </c>
+      <c r="AX51" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>23,</v>
+      </c>
+      <c r="AY51" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>23,</v>
+      </c>
+      <c r="AZ51" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>23,</v>
+      </c>
+      <c r="BA51" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>23,</v>
+      </c>
+      <c r="BB51" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>23,</v>
+      </c>
+      <c r="BC51" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>23,</v>
+      </c>
+      <c r="BD51" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>23,</v>
+      </c>
+      <c r="BE51" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>23,</v>
+      </c>
+      <c r="BF51" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>23,</v>
+      </c>
+      <c r="BG51" s="1" t="str">
+        <f t="shared" si="11"/>
+        <v>23,</v>
+      </c>
+      <c r="BH51" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>23,</v>
+      </c>
+      <c r="BI51" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>23,</v>
+      </c>
+      <c r="BJ51" s="1">
+        <f t="shared" si="17"/>
+        <v>23</v>
+      </c>
+      <c r="BK51" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>23},</v>
+      </c>
     </row>
-    <row r="53" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:63" x14ac:dyDescent="0.25">
       <c r="AA53" s="1"/>
+      <c r="AF53" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="54" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:63" x14ac:dyDescent="0.25">
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:63" x14ac:dyDescent="0.25">
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:63" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AA56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="57" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:63" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="D59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="D60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I57" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C63" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="D63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="3:63" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z57" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C58" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA58" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA59" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C60" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA60" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C61" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z61" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA61" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C62" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z62" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C63" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z63" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA63" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C64" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z64" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z66" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z67" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z68" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="X69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Y69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z69" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="3:27" x14ac:dyDescent="0.25">

</xml_diff>